<commit_message>
further updates to jupyter notebook code
</commit_message>
<xml_diff>
--- a/State of Childcare Survey.xlsx
+++ b/State of Childcare Survey.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swanson/Projects/4CforChildren/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B8CB89-85C2-EF4C-BBCB-AEA219D83858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0DC344-B5C3-C44A-A522-7194DF4C10B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="38160" windowHeight="19140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$CV$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5448" uniqueCount="1381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5448" uniqueCount="1407">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -4138,31 +4141,109 @@
     <t>email</t>
   </si>
   <si>
-    <t># of Classrooms not open</t>
-  </si>
-  <si>
-    <t># of staff needed to open these classrooms</t>
-  </si>
-  <si>
-    <t># of Children that could be served in these currently unopened classrooms</t>
-  </si>
-  <si>
     <t>Do you have any classrooms that are not at full capacity because of a shortage of staff?</t>
   </si>
   <si>
-    <t># of Children that could be served in these currently unopened/limited classrooms</t>
-  </si>
-  <si>
-    <t>What is your current enrollment?</t>
-  </si>
-  <si>
-    <t>What is your ideal enrollment?</t>
-  </si>
-  <si>
-    <t>Which populations are you serving or did you serve? Check all that apply.</t>
-  </si>
-  <si>
-    <t>Which populations are you serving or have previously served?</t>
+    <t>What is your current enrollment?-Infants</t>
+  </si>
+  <si>
+    <t>What is your current enrollment?-Toddlers</t>
+  </si>
+  <si>
+    <t>What is your current enrollment?-School Age</t>
+  </si>
+  <si>
+    <t>What is your current enrollment?-Preschool</t>
+  </si>
+  <si>
+    <t>What is your ideal enrollment?-Infants</t>
+  </si>
+  <si>
+    <t>What is your ideal enrollment?-Toddlers</t>
+  </si>
+  <si>
+    <t>What is your ideal enrollment?-Preschool</t>
+  </si>
+  <si>
+    <t>What is your ideal enrollment?-School Age</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or did you serve?-English Language Learner</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or did you serve?-Children Experiencing Homelessness</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or did you serve?-Children with Special Needs</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or did you serve?-Infants and/or Toddlers</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or have previously served?-Children with Special Needs</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or have previously served?-Children Experiencing Homelessness</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or have previously served?-Infants or Toddlers</t>
+  </si>
+  <si>
+    <t>Which populations are you serving or have previously served?-English Language Learner</t>
+  </si>
+  <si>
+    <t>classrooms not open-Infant</t>
+  </si>
+  <si>
+    <t>classrooms not open-Toddler</t>
+  </si>
+  <si>
+    <t>classrooms not open-Preschool</t>
+  </si>
+  <si>
+    <t>classrooms not open-School Age</t>
+  </si>
+  <si>
+    <t>staff needed to open these classrooms-Infant</t>
+  </si>
+  <si>
+    <t>staff needed to open these classrooms-Toddler</t>
+  </si>
+  <si>
+    <t>of staff needed to open these classrooms-Preschool</t>
+  </si>
+  <si>
+    <t>of staff needed to open these classrooms-School Age</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened classrooms-Infant</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened classrooms-Toddler</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened classrooms-Preschool</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened classrooms-School Age</t>
+  </si>
+  <si>
+    <t>staff needed to open these classrooms-Preschool</t>
+  </si>
+  <si>
+    <t>staff needed to open these classrooms-School Age</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened/limited classrooms-Toddler</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened/limited classrooms-Infant</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened/limited classrooms-Preschool</t>
+  </si>
+  <si>
+    <t>children that could be served in these currently unopened/limited classrooms-School Age</t>
   </si>
 </sst>
 </file>
@@ -4569,8 +4650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CV316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" topLeftCell="CQ1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4585,7 +4666,7 @@
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="76.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.83203125" style="4" customWidth="1"/>
     <col min="13" max="13" width="22.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="47.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="22.6640625" style="6" bestFit="1" customWidth="1"/>
@@ -4637,7 +4718,7 @@
     <col min="86" max="86" width="37.1640625" bestFit="1" customWidth="1"/>
     <col min="87" max="87" width="71" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="203.33203125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="187.83203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="56.5" customWidth="1"/>
     <col min="90" max="93" width="53.6640625" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="106.6640625" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="255.83203125" bestFit="1" customWidth="1"/>
@@ -4683,103 +4764,103 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>1389</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>1390</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>1395</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>1397</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>1400</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>1372</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="P1" s="7" t="s">
+      <c r="Y1" s="5" t="s">
+        <v>1389</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>1390</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>1393</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>1394</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>1401</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>1402</v>
+      </c>
+      <c r="AG1" s="9" t="s">
+        <v>1404</v>
+      </c>
+      <c r="AH1" s="9" t="s">
+        <v>1403</v>
+      </c>
+      <c r="AI1" s="9" t="s">
+        <v>1405</v>
+      </c>
+      <c r="AJ1" s="9" t="s">
+        <v>1406</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>1373</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>1374</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>1374</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>1374</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>1374</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>1375</v>
       </c>
-      <c r="Y1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>1372</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>1373</v>
-      </c>
-      <c r="AG1" s="9" t="s">
-        <v>1376</v>
-      </c>
-      <c r="AH1" s="9" t="s">
-        <v>1376</v>
-      </c>
-      <c r="AI1" s="9" t="s">
-        <v>1376</v>
-      </c>
-      <c r="AJ1" s="9" t="s">
-        <v>1376</v>
-      </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>1377</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>1377</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>1377</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>1377</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>1378</v>
       </c>
       <c r="AP1" s="2" t="s">
         <v>1378</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="AS1" s="2" t="s">
         <v>11</v>
@@ -4830,43 +4911,43 @@
         <v>25</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>1379</v>
+        <v>1382</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>1379</v>
+        <v>1383</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>1379</v>
+        <v>1384</v>
       </c>
       <c r="BM1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="BN1" s="7" t="s">
+        <v>1373</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>1376</v>
+      </c>
+      <c r="BQ1" s="7" t="s">
+        <v>1375</v>
+      </c>
+      <c r="BR1" s="7" t="s">
         <v>1377</v>
-      </c>
-      <c r="BO1" s="7" t="s">
-        <v>1377</v>
-      </c>
-      <c r="BP1" s="7" t="s">
-        <v>1377</v>
-      </c>
-      <c r="BQ1" s="7" t="s">
-        <v>1377</v>
-      </c>
-      <c r="BR1" s="7" t="s">
-        <v>1378</v>
       </c>
       <c r="BS1" s="7" t="s">
         <v>1378</v>
       </c>
       <c r="BT1" s="7" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="BU1" s="7" t="s">
-        <v>1378</v>
+        <v>1380</v>
       </c>
       <c r="BV1" s="2" t="s">
         <v>11</v>
@@ -4917,16 +4998,16 @@
         <v>31</v>
       </c>
       <c r="CL1" s="2" t="s">
-        <v>1380</v>
+        <v>1388</v>
       </c>
       <c r="CM1" s="2" t="s">
-        <v>1380</v>
+        <v>1386</v>
       </c>
       <c r="CN1" s="2" t="s">
-        <v>1380</v>
+        <v>1385</v>
       </c>
       <c r="CO1" s="2" t="s">
-        <v>1380</v>
+        <v>1387</v>
       </c>
       <c r="CP1" s="2" t="s">
         <v>32</v>

</xml_diff>